<commit_message>
Created combined PRD for ATR 72-600 and A220-100 showing flight data for US market
</commit_message>
<xml_diff>
--- a/nils/pr_data_ref_ac.xlsx
+++ b/nils/pr_data_ref_ac.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmb48\Documents\GitHub\eurocontrol-data-archive\nils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39B508DB-D237-4249-9A82-1BFA3E71FB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD2DBAA-09A8-4428-B9AC-555D23B0282D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5145" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{80E6A51D-45AC-4AC3-824D-41944F122555}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{80E6A51D-45AC-4AC3-824D-41944F122555}"/>
   </bookViews>
   <sheets>
-    <sheet name="ATR 72-600" sheetId="1" r:id="rId1"/>
-    <sheet name="A220-300" sheetId="2" r:id="rId2"/>
-    <sheet name="A320 neo" sheetId="3" r:id="rId3"/>
+    <sheet name="ATR 72-600_pax" sheetId="1" r:id="rId1"/>
+    <sheet name="ATR 72-600" sheetId="5" r:id="rId2"/>
+    <sheet name="A220-300" sheetId="2" r:id="rId3"/>
+    <sheet name="A220-100" sheetId="4" r:id="rId4"/>
+    <sheet name="A320 neo" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +39,80 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A83D895D-81E7-4A3B-9723-8F7494F9C625}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A83D895D-81E7-4A3B-9723-8F7494F9C625}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Data from figure 9 in high_whitepaper_2023_perFCretroac_mukhopadhaya, see "C:\Users\nmb48\Documents\GitHub\Flydrogen\misc\fyr\FYR_DigitGraph_Data\fig9_mukhopadhaya_LH2_yellow.csv"</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B3144F75-EE38-4A93-A746-4630B9AC3542}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B3144F75-EE38-4A93-A746-4630B9AC3542}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Data from figure 79 in "C:\Users\nmb48\OneDrive - University of Cambridge\Desktop\PhD\Literature\2nd Year\Reports\Restricted FlyZero Reports\FZO-AIN-REP-0008 - Regional Aircraft Concept Report.pdf"</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={07A65DD4-2BF7-4A3D-B979-4725B3CD353A}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{07A65DD4-2BF7-4A3D-B979-4725B3CD353A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Data from page 223 in A220-ACP-Issue011-00-18Sep2025</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A631AD09-5793-4681-B3F0-76E709422FA1}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A631AD09-5793-4681-B3F0-76E709422FA1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Data from page 209 in A220-ACP-Issue011-00-18Sep2025</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="3">
   <si>
     <t>x</t>
   </si>
@@ -101,10 +175,16 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Nils Barner" id="{21094F57-5877-4A47-9AFA-381D356CB492}" userId="S::nmb48@cam.ac.uk::587eb34a-3ad7-4082-8972-e826c31cd372" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +222,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -248,7 +328,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -390,23 +470,67 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2026-02-02T20:32:26.65" personId="{21094F57-5877-4A47-9AFA-381D356CB492}" id="{A83D895D-81E7-4A3B-9723-8F7494F9C625}">
+    <text>Data from figure 9 in high_whitepaper_2023_perFCretroac_mukhopadhaya, see "C:\Users\nmb48\Documents\GitHub\Flydrogen\misc\fyr\FYR_DigitGraph_Data\fig9_mukhopadhaya_LH2_yellow.csv"</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>1909648331</xltc2:checksum>
+        <xltc2:hyperlink startIndex="75" length="103" url="C:\Users\nmb48\Documents\GitHub\Flydrogen\misc\fyr\FYR_DigitGraph_Data\fig9_mukhopadhaya_LH2_yellow.csv"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2026-02-02T20:52:22.36" personId="{21094F57-5877-4A47-9AFA-381D356CB492}" id="{B3144F75-EE38-4A93-A746-4630B9AC3542}">
+    <text>Data from figure 79 in "C:\Users\nmb48\OneDrive - University of Cambridge\Desktop\PhD\Literature\2nd Year\Reports\Restricted FlyZero Reports\FZO-AIN-REP-0008 - Regional Aircraft Concept Report.pdf"</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>2906974973</xltc2:checksum>
+        <xltc2:hyperlink startIndex="24" length="172" url="C:\Users\nmb48\OneDrive - University of Cambridge\Desktop\PhD\Literature\2nd Year\Reports\Restricted FlyZero Reports\FZO-AIN-REP-0008 - Regional Aircraft Concept Report.pdf"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2026-02-02T16:07:35.15" personId="{21094F57-5877-4A47-9AFA-381D356CB492}" id="{07A65DD4-2BF7-4A3D-B979-4725B3CD353A}">
+    <text>Data from page 223 in A220-ACP-Issue011-00-18Sep2025</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2026-02-02T16:06:33.43" personId="{21094F57-5877-4A47-9AFA-381D356CB492}" id="{A631AD09-5793-4681-B3F0-76E709422FA1}">
+    <text>Data from page 209 in A220-ACP-Issue011-00-18Sep2025</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8DA57C-55FD-4F9F-BE88-CDED6E7B6CDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8DA57C-55FD-4F9F-BE88-CDED6E7B6CDA}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -422,7 +546,7 @@
         <v>77.938722484723598</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1148.14819335937</v>
       </c>
@@ -430,7 +554,7 @@
         <v>77.938722484723598</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3455.5558268229101</v>
       </c>
@@ -438,7 +562,7 @@
         <v>46.740950016125602</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3714.8148600260402</v>
       </c>
@@ -448,20 +572,169 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912D1139-50D2-4F15-B476-3A37FF13B071}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58800F09-F505-4BE1-9742-6C0704FA377D}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2.8571428571427702</v>
+      </c>
+      <c r="B2">
+        <v>7323.1132075471696</v>
+      </c>
+      <c r="D2">
+        <v>2.8571428571427702</v>
+      </c>
+      <c r="E2">
+        <v>7323.1132075471696</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>408.57142857142799</v>
+      </c>
+      <c r="B3">
+        <v>7334.9056603773597</v>
+      </c>
+      <c r="D3">
+        <v>408.57142857142799</v>
+      </c>
+      <c r="E3">
+        <v>7334.9056603773597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>825.71428571428498</v>
+      </c>
+      <c r="B4">
+        <v>6344.3396226415098</v>
+      </c>
+      <c r="D4">
+        <v>739.99999999999898</v>
+      </c>
+      <c r="E4">
+        <v>6544.8113207547103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1639.99999999999</v>
+      </c>
+      <c r="B5">
+        <v>4375</v>
+      </c>
+      <c r="D5">
+        <v>1639.99999999999</v>
+      </c>
+      <c r="E5">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1751.42857142857</v>
+      </c>
+      <c r="B6">
+        <v>23.5849056603783</v>
+      </c>
+      <c r="D6">
+        <v>1751.42857142857</v>
+      </c>
+      <c r="E6">
+        <v>23.5849056603783</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912D1139-50D2-4F15-B476-3A37FF13B071}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>128.00892174370901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2146.4449232811098</v>
+      </c>
+      <c r="B3">
+        <v>128.024238679202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3213.17696200406</v>
+      </c>
+      <c r="B4">
+        <v>118.14068279723099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3860.4305646535099</v>
+      </c>
+      <c r="B5">
+        <v>94.059664089667393</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885B91AE-0425-455D-9786-0745713F1E41}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,44 +742,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.15933724842275801</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>128.00892174370901</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>115.992957746478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2146.4449232811098</v>
+        <v>956.15514333895396</v>
       </c>
       <c r="B3">
-        <v>128.024238679202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>115.948356807511</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3213.17696200406</v>
+        <v>2098.2293423271499</v>
       </c>
       <c r="B4">
-        <v>118.14068279723099</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>115.45774647887301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3860.4305646535099</v>
+        <v>3430.0168634063998</v>
       </c>
       <c r="B5">
-        <v>94.059664089667393</v>
+        <v>104.530516431924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3771.50084317032</v>
+      </c>
+      <c r="B6">
+        <v>101.85446009389599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4435.4974704890301</v>
+      </c>
+      <c r="B7">
+        <v>80.044600938967093</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43EF2AF-0B32-49B4-9ADA-B05BF59CC2F1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -514,9 +804,9 @@
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-2.8457598178713699</v>
       </c>
@@ -532,7 +822,7 @@
         <v>19425.6756756756</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2492.8856004553199</v>
       </c>
@@ -540,7 +830,7 @@
         <v>19377.4131274131</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3497.4388161639099</v>
       </c>
@@ -548,7 +838,7 @@
         <v>14502.8957528957</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4393.8531587933903</v>
       </c>

</xml_diff>

<commit_message>
Merge with 4-months-old stale changes on CDT laptop
</commit_message>
<xml_diff>
--- a/nils/pr_data_ref_ac.xlsx
+++ b/nils/pr_data_ref_ac.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmb48\Documents\GitHub\eurocontrol-data-archive\nils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/nmb48_cam_ac_uk/Documents/Documents/GitHub/eurocontrol-data-archive/nils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39B508DB-D237-4249-9A82-1BFA3E71FB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{39B508DB-D237-4249-9A82-1BFA3E71FB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6BF31F4-1AE4-461F-A8BC-5A012A9BB966}"/>
   <bookViews>
-    <workbookView xWindow="-5145" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{80E6A51D-45AC-4AC3-824D-41944F122555}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{80E6A51D-45AC-4AC3-824D-41944F122555}"/>
   </bookViews>
   <sheets>
     <sheet name="ATR 72-600" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +142,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -248,7 +248,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -390,7 +390,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -400,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8DA57C-55FD-4F9F-BE88-CDED6E7B6CDA}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912D1139-50D2-4F15-B476-3A37FF13B071}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,7 +471,8 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.15933724842275801</v>
+        <f>0.159337248422758*1.852</f>
+        <v>0.29509258407894784</v>
       </c>
       <c r="B2">
         <v>128.00892174370901</v>
@@ -479,7 +480,8 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2146.4449232811098</v>
+        <f>2146.44492328111*1.852</f>
+        <v>3975.2159979166154</v>
       </c>
       <c r="B3">
         <v>128.024238679202</v>
@@ -487,7 +489,8 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3213.17696200406</v>
+        <f>3213.17696200406*1.852</f>
+        <v>5950.8037336315192</v>
       </c>
       <c r="B4">
         <v>118.14068279723099</v>
@@ -495,7 +498,8 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3860.4305646535099</v>
+        <f>3860.43056465351*1.852</f>
+        <v>7149.517405738301</v>
       </c>
       <c r="B5">
         <v>94.059664089667393</v>
@@ -511,7 +515,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,7 +530,8 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>-2.8457598178713699</v>
+        <f>-2.84575981787137*1.852</f>
+        <v>-5.270347182697777</v>
       </c>
       <c r="B2">
         <v>19425.6756756756</v>
@@ -534,7 +539,8 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2492.8856004553199</v>
+        <f>2492.88560045532*1.852</f>
+        <v>4616.8241320432526</v>
       </c>
       <c r="B3">
         <v>19377.4131274131</v>
@@ -542,7 +548,8 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3497.4388161639099</v>
+        <f>3497.43881616391*1.852</f>
+        <v>6477.2566875355615</v>
       </c>
       <c r="B4">
         <v>14502.8957528957</v>
@@ -550,7 +557,8 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4393.8531587933903</v>
+        <f>4393.85315879339*1.852</f>
+        <v>8137.4160500853595</v>
       </c>
       <c r="B5">
         <v>48.262548262548201</v>

</xml_diff>